<commit_message>
added new CPJ template and changed layout of link to download templates
</commit_message>
<xml_diff>
--- a/Documents/CASH RECEIPTS JOURNAL TEMPLATE.xlsx
+++ b/Documents/CASH RECEIPTS JOURNAL TEMPLATE.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF74BB85-1DBB-A544-840D-6C132D812100}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA15305-D98B-D942-B12A-94CC49EEDDDE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">CASH RECEIPTS JOURNAL OF </t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME: </t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -454,6 +457,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,26 +495,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,26 +811,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C8F528-2091-174E-98F3-CF5C80FBA67B}">
-  <dimension ref="A1:S38"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="6.83203125" customWidth="1"/>
     <col min="11" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -846,20 +855,20 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="11" t="s">
-        <v>0</v>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -869,18 +878,18 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -890,34 +899,20 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="17" t="s">
-        <v>1</v>
+      <c r="B4" s="25" t="s">
+        <v>0</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -927,28 +922,18 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>3</v>
-      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -958,18 +943,34 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -979,18 +980,28 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="4"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>3</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1002,16 +1013,16 @@
     </row>
     <row r="8" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1027,10 +1038,10 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
       <c r="L9" s="1"/>
@@ -1048,7 +1059,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1273,18 +1284,18 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1296,16 +1307,16 @@
     </row>
     <row r="22" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="4"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1315,18 +1326,18 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="7"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1651,11 +1662,54 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
+    <row r="39" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B4:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new table feature and creation of solution started
</commit_message>
<xml_diff>
--- a/Documents/CASH RECEIPTS JOURNAL TEMPLATE.xlsx
+++ b/Documents/CASH RECEIPTS JOURNAL TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09C70C-053F-AD48-AA21-3F913193DAF6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0958110A-8B9B-FD45-A7BC-E64374621077}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">CASH RECEIPTS JOURNAL OF </t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Receipts</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Income</t>
   </si>
   <si>
     <t xml:space="preserve">NAME: </t>
@@ -480,22 +474,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,8 +810,8 @@
   </sheetPr>
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +854,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -963,9 +957,7 @@
       <c r="G6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="24" t="s">
         <v>7</v>
       </c>
@@ -990,9 +982,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="H7" s="16"/>
       <c r="I7" s="19" t="s">
         <v>5</v>
       </c>

</xml_diff>